<commit_message>
Add files loaded from disk to unit tests
</commit_message>
<xml_diff>
--- a/Data/Test1.xlsx
+++ b/Data/Test1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Test Field</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Test Name C</t>
   </si>
   <si>
-    <t>Still Another Test Name</t>
-  </si>
-  <si>
     <t>This is a simple test.</t>
   </si>
   <si>
@@ -40,15 +37,6 @@
   </si>
   <si>
     <t>Even more tests of text</t>
-  </si>
-  <si>
-    <t>Still more text</t>
-  </si>
-  <si>
-    <t>Yet Another Test Name</t>
-  </si>
-  <si>
-    <t>Yet more text to test</t>
   </si>
   <si>
     <t>Integer Field</t>
@@ -396,11 +384,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -413,13 +399,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -436,7 +422,7 @@
         <v>4.5</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -450,7 +436,7 @@
         <v>123.456</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,35 +450,7 @@
         <v>22.334499999999998</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>1.5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>99.99</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes and more comprehensive documentation
</commit_message>
<xml_diff>
--- a/Data/Test1.xlsx
+++ b/Data/Test1.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Test Field</t>
-  </si>
-  <si>
     <t>Test Name A</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Name Field</t>
+  </si>
+  <si>
+    <t>Text Field</t>
   </si>
 </sst>
 </file>
@@ -95,6 +95,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name Field"/>
+    <tableColumn id="2" name="Integer Field"/>
+    <tableColumn id="3" name="Float Field"/>
+    <tableColumn id="4" name="Text Field"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,34 +399,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -422,12 +437,12 @@
         <v>4.5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -436,12 +451,12 @@
         <v>123.456</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -450,11 +465,14 @@
         <v>22.334499999999998</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>